<commit_message>
added excel reader, testNG and waits
</commit_message>
<xml_diff>
--- a/data/testdata.xlsx
+++ b/data/testdata.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3f159fc1f1f3909f/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8B76A48-9CBE-4211-8E2F-33105840D4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{7762FB33-81E2-4D71-983A-CB6F47960285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A33152E-A14E-4591-8300-A4D0F4A45456}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +23,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,9 +35,6 @@
     <t>firstname</t>
   </si>
   <si>
-    <t>lastnam,e</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -62,6 +54,9 @@
   </si>
   <si>
     <t>bhabani@test.com</t>
+  </si>
+  <si>
+    <t>lastname</t>
   </si>
 </sst>
 </file>
@@ -111,8 +106,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +425,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -440,34 +435,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="1"/>
     </row>

</xml_diff>